<commit_message>
Add Contact_Me.py and sending email function
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -509,12 +509,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>7:50pm</t>
+          <t>7:35am</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>3</t>
         </is>
       </c>
     </row>

</xml_diff>